<commit_message>
Synthesized 500 voiceless and 500 voiced training wav files. Some of the voiceless tokens don't sound voiceless and some non-bilabial stops sound bilabial; I included some notes on this
</commit_message>
<xml_diff>
--- a/klatt_synthesis/sample_klatt_params.xlsx
+++ b/klatt_synthesis/sample_klatt_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hughe\Documents\CNN_Perceptual_Integration_Channel_Bias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1486A45-078B-4A53-9C0F-1255DE65BF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E0BB77-E1DF-4FA3-AB9D-18FFAA005458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{06E8A5E1-E3B5-42F4-B76E-CFCEADA3CE17}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -97,10 +97,37 @@
     <t>VowelDur</t>
   </si>
   <si>
-    <t>HighF1LongClosure</t>
-  </si>
-  <si>
     <t>f0TransitionDur</t>
+  </si>
+  <si>
+    <t>HighF1_LongClosure_Highf0</t>
+  </si>
+  <si>
+    <t>HighF1_ShortClosure_Highf0</t>
+  </si>
+  <si>
+    <t>LowF1_LongClosure_Highf0</t>
+  </si>
+  <si>
+    <t>LowF1_ShortClosure_Highf0</t>
+  </si>
+  <si>
+    <t>HighF1_LongClosure_Lowf0</t>
+  </si>
+  <si>
+    <t>HighF1_ShortClosure_Lowf0</t>
+  </si>
+  <si>
+    <t>LowF1_LongClosure_Lowf0</t>
+  </si>
+  <si>
+    <t>LowF1_ShortClosure_Lowf0</t>
+  </si>
+  <si>
+    <t>HighF1_LongVoicing</t>
+  </si>
+  <si>
+    <t>HighF1_ShortVoicing</t>
   </si>
 </sst>
 </file>
@@ -116,12 +143,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,8 +169,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDA1EC8-BB40-42D4-B129-E5A460CAB0DE}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,7 +541,7 @@
         <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q1" t="s">
         <v>13</v>
@@ -527,7 +561,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>0.20499999999999999</v>
@@ -588,6 +622,567 @@
       </c>
       <c r="U2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.03</v>
+      </c>
+      <c r="D3">
+        <v>450</v>
+      </c>
+      <c r="E3">
+        <v>800</v>
+      </c>
+      <c r="F3">
+        <v>800</v>
+      </c>
+      <c r="G3">
+        <v>1150</v>
+      </c>
+      <c r="H3">
+        <v>1750</v>
+      </c>
+      <c r="I3">
+        <v>2400</v>
+      </c>
+      <c r="J3">
+        <v>3300</v>
+      </c>
+      <c r="K3">
+        <v>3300</v>
+      </c>
+      <c r="L3">
+        <v>3850</v>
+      </c>
+      <c r="M3">
+        <v>3850</v>
+      </c>
+      <c r="N3">
+        <v>130</v>
+      </c>
+      <c r="O3">
+        <v>130</v>
+      </c>
+      <c r="P3">
+        <v>0.04</v>
+      </c>
+      <c r="Q3">
+        <v>0.04</v>
+      </c>
+      <c r="R3">
+        <v>0.04</v>
+      </c>
+      <c r="S3">
+        <v>450</v>
+      </c>
+      <c r="T3">
+        <v>130</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D4">
+        <v>150</v>
+      </c>
+      <c r="E4">
+        <v>800</v>
+      </c>
+      <c r="F4">
+        <v>800</v>
+      </c>
+      <c r="G4">
+        <v>1150</v>
+      </c>
+      <c r="H4">
+        <v>1750</v>
+      </c>
+      <c r="I4">
+        <v>2400</v>
+      </c>
+      <c r="J4">
+        <v>3300</v>
+      </c>
+      <c r="K4">
+        <v>3300</v>
+      </c>
+      <c r="L4">
+        <v>3850</v>
+      </c>
+      <c r="M4">
+        <v>3850</v>
+      </c>
+      <c r="N4">
+        <v>130</v>
+      </c>
+      <c r="O4">
+        <v>130</v>
+      </c>
+      <c r="P4">
+        <v>0.04</v>
+      </c>
+      <c r="Q4">
+        <v>0.04</v>
+      </c>
+      <c r="R4">
+        <v>0.04</v>
+      </c>
+      <c r="S4">
+        <v>450</v>
+      </c>
+      <c r="T4">
+        <v>130</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.03</v>
+      </c>
+      <c r="D5">
+        <v>150</v>
+      </c>
+      <c r="E5">
+        <v>800</v>
+      </c>
+      <c r="F5">
+        <v>800</v>
+      </c>
+      <c r="G5">
+        <v>1150</v>
+      </c>
+      <c r="H5">
+        <v>1750</v>
+      </c>
+      <c r="I5">
+        <v>2400</v>
+      </c>
+      <c r="J5">
+        <v>3300</v>
+      </c>
+      <c r="K5">
+        <v>3300</v>
+      </c>
+      <c r="L5">
+        <v>3850</v>
+      </c>
+      <c r="M5">
+        <v>3850</v>
+      </c>
+      <c r="N5">
+        <v>130</v>
+      </c>
+      <c r="O5">
+        <v>130</v>
+      </c>
+      <c r="P5">
+        <v>0.04</v>
+      </c>
+      <c r="Q5">
+        <v>0.04</v>
+      </c>
+      <c r="R5">
+        <v>0.04</v>
+      </c>
+      <c r="S5">
+        <v>450</v>
+      </c>
+      <c r="T5">
+        <v>130</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D6">
+        <v>450</v>
+      </c>
+      <c r="E6">
+        <v>800</v>
+      </c>
+      <c r="F6">
+        <v>800</v>
+      </c>
+      <c r="G6">
+        <v>1150</v>
+      </c>
+      <c r="H6">
+        <v>1750</v>
+      </c>
+      <c r="I6">
+        <v>2400</v>
+      </c>
+      <c r="J6">
+        <v>3300</v>
+      </c>
+      <c r="K6">
+        <v>3300</v>
+      </c>
+      <c r="L6">
+        <v>3850</v>
+      </c>
+      <c r="M6">
+        <v>3850</v>
+      </c>
+      <c r="N6">
+        <v>90</v>
+      </c>
+      <c r="O6">
+        <v>90</v>
+      </c>
+      <c r="P6">
+        <v>0.04</v>
+      </c>
+      <c r="Q6">
+        <v>0.04</v>
+      </c>
+      <c r="R6">
+        <v>0.04</v>
+      </c>
+      <c r="S6">
+        <v>450</v>
+      </c>
+      <c r="T6">
+        <v>90</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.03</v>
+      </c>
+      <c r="D7">
+        <v>450</v>
+      </c>
+      <c r="E7">
+        <v>800</v>
+      </c>
+      <c r="F7">
+        <v>800</v>
+      </c>
+      <c r="G7">
+        <v>1150</v>
+      </c>
+      <c r="H7">
+        <v>1750</v>
+      </c>
+      <c r="I7">
+        <v>2400</v>
+      </c>
+      <c r="J7">
+        <v>3300</v>
+      </c>
+      <c r="K7">
+        <v>3300</v>
+      </c>
+      <c r="L7">
+        <v>3850</v>
+      </c>
+      <c r="M7">
+        <v>3850</v>
+      </c>
+      <c r="N7">
+        <v>90</v>
+      </c>
+      <c r="O7">
+        <v>90</v>
+      </c>
+      <c r="P7">
+        <v>0.04</v>
+      </c>
+      <c r="Q7">
+        <v>0.04</v>
+      </c>
+      <c r="R7">
+        <v>0.04</v>
+      </c>
+      <c r="S7">
+        <v>450</v>
+      </c>
+      <c r="T7">
+        <v>90</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D8">
+        <v>150</v>
+      </c>
+      <c r="E8">
+        <v>800</v>
+      </c>
+      <c r="F8">
+        <v>800</v>
+      </c>
+      <c r="G8">
+        <v>1150</v>
+      </c>
+      <c r="H8">
+        <v>1750</v>
+      </c>
+      <c r="I8">
+        <v>2400</v>
+      </c>
+      <c r="J8">
+        <v>3300</v>
+      </c>
+      <c r="K8">
+        <v>3300</v>
+      </c>
+      <c r="L8">
+        <v>3850</v>
+      </c>
+      <c r="M8">
+        <v>3850</v>
+      </c>
+      <c r="N8">
+        <v>90</v>
+      </c>
+      <c r="O8">
+        <v>90</v>
+      </c>
+      <c r="P8">
+        <v>0.04</v>
+      </c>
+      <c r="Q8">
+        <v>0.04</v>
+      </c>
+      <c r="R8">
+        <v>0.04</v>
+      </c>
+      <c r="S8">
+        <v>450</v>
+      </c>
+      <c r="T8">
+        <v>90</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C9">
+        <v>0.03</v>
+      </c>
+      <c r="D9">
+        <v>150</v>
+      </c>
+      <c r="E9">
+        <v>800</v>
+      </c>
+      <c r="F9">
+        <v>800</v>
+      </c>
+      <c r="G9">
+        <v>1150</v>
+      </c>
+      <c r="H9">
+        <v>1750</v>
+      </c>
+      <c r="I9">
+        <v>2400</v>
+      </c>
+      <c r="J9">
+        <v>3300</v>
+      </c>
+      <c r="K9">
+        <v>3300</v>
+      </c>
+      <c r="L9">
+        <v>3850</v>
+      </c>
+      <c r="M9">
+        <v>3850</v>
+      </c>
+      <c r="N9">
+        <v>90</v>
+      </c>
+      <c r="O9">
+        <v>90</v>
+      </c>
+      <c r="P9">
+        <v>0.04</v>
+      </c>
+      <c r="Q9">
+        <v>0.04</v>
+      </c>
+      <c r="R9">
+        <v>0.04</v>
+      </c>
+      <c r="S9">
+        <v>450</v>
+      </c>
+      <c r="T9">
+        <v>90</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.08</v>
+      </c>
+      <c r="D10">
+        <v>400</v>
+      </c>
+      <c r="E10">
+        <v>750</v>
+      </c>
+      <c r="F10">
+        <v>800</v>
+      </c>
+      <c r="G10">
+        <v>1150</v>
+      </c>
+      <c r="H10">
+        <v>1750</v>
+      </c>
+      <c r="I10">
+        <v>2400</v>
+      </c>
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10">
+        <v>100</v>
+      </c>
+      <c r="P10" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="Q10">
+        <v>5.5E-2</v>
+      </c>
+      <c r="R10">
+        <v>0.04</v>
+      </c>
+      <c r="S10">
+        <v>150</v>
+      </c>
+      <c r="T10">
+        <v>90</v>
+      </c>
+      <c r="U10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.08</v>
+      </c>
+      <c r="D11">
+        <v>400</v>
+      </c>
+      <c r="E11">
+        <v>750</v>
+      </c>
+      <c r="F11">
+        <v>800</v>
+      </c>
+      <c r="G11">
+        <v>1150</v>
+      </c>
+      <c r="H11">
+        <v>1750</v>
+      </c>
+      <c r="I11">
+        <v>2400</v>
+      </c>
+      <c r="N11">
+        <v>100</v>
+      </c>
+      <c r="O11">
+        <v>100</v>
+      </c>
+      <c r="P11" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="Q11">
+        <v>5.5E-2</v>
+      </c>
+      <c r="R11">
+        <v>0.04</v>
+      </c>
+      <c r="S11">
+        <v>150</v>
+      </c>
+      <c r="T11">
+        <v>90</v>
+      </c>
+      <c r="U11">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>